<commit_message>
en papulandia habiaun papu
un papu pro un papu pro
</commit_message>
<xml_diff>
--- a/docs/Animaciones.xlsx
+++ b/docs/Animaciones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LAGS-heartbeat\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chemi\Documents\GitHub\LAGS-heartbeat\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43DDACFE-B7D2-4BFE-A925-D9EDF0145568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9CA1B3-18F5-46FF-BD49-E8A1066E034D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11790" xr2:uid="{C8BCF65A-ACDE-4379-BB17-E744033FB16C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C8BCF65A-ACDE-4379-BB17-E744033FB16C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Enemigos</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Hecho</t>
+  </si>
+  <si>
+    <t>Stunned</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -127,19 +130,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,7 +201,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -480,23 +517,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B50513E-5692-478C-BDE7-5B8704F9C436}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="146" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -507,55 +545,62 @@
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="2" t="s">
+      <c r="E4" s="3"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="2" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>